<commit_message>
Das Bearbeiten von IPTC Titel und BEschreibung funktioniert
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6923A2-8A55-4641-A35D-4368AB2E8B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="1870" yWindow="0" windowWidth="18280" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notenrechner" sheetId="2" r:id="rId1"/>
@@ -14,7 +15,17 @@
     <definedName name="Studenten">#REF!</definedName>
     <definedName name="TabelleNotenTest">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -135,9 +146,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -318,7 +329,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -352,8 +363,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -369,10 +380,10 @@
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
     <cellStyle name="Ergebnis" xfId="5" builtinId="25"/>
     <cellStyle name="Komma" xfId="8" builtinId="3"/>
-    <cellStyle name="Normal_Noten" xfId="6"/>
+    <cellStyle name="Normal_Noten" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Notiz" xfId="4" builtinId="10"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="7"/>
+    <cellStyle name="Standard 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
     <cellStyle name="Überschrift 2" xfId="2" builtinId="17"/>
   </cellStyles>
@@ -390,7 +401,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -512,6 +523,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-663C-44E5-B574-B65667601967}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -612,6 +628,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-663C-44E5-B574-B65667601967}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -762,7 +783,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -781,7 +808,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -856,6 +883,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -891,6 +935,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1066,24 +1127,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="75.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="22" t="s">
         <v>8</v>
       </c>
@@ -1091,12 +1152,12 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1110,33 +1171,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -1146,7 +1211,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
@@ -1156,17 +1221,19 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
       <c r="C10" s="7">
         <v>2</v>
       </c>
       <c r="D10" s="14"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
@@ -1176,15 +1243,15 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>24</v>
       </c>
@@ -1194,7 +1261,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
@@ -1204,7 +1271,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1214,7 +1281,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -1224,7 +1291,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>34</v>
       </c>
@@ -1234,15 +1301,15 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>30</v>
       </c>
@@ -1252,7 +1319,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>31</v>
       </c>
@@ -1262,15 +1329,15 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
@@ -1280,7 +1347,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>32</v>
       </c>
@@ -1290,7 +1357,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
@@ -1300,15 +1367,15 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1383,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>6</v>
       </c>
@@ -1324,7 +1391,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>11</v>
       </c>
@@ -1332,20 +1399,20 @@
       <c r="C32" s="7"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -1356,19 +1423,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="15"/>
+    <col min="1" max="1" width="10.7265625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
@@ -1376,7 +1443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="15">
         <v>42.5</v>
       </c>
@@ -1384,7 +1451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>39.5</v>
       </c>
@@ -1392,7 +1459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>77</v>
       </c>
@@ -1400,7 +1467,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>92</v>
       </c>
@@ -1408,7 +1475,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="15">
         <v>93</v>
       </c>
@@ -1416,7 +1483,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>66</v>
       </c>
@@ -1433,7 +1500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>81</v>
       </c>
@@ -1450,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>62.5</v>
       </c>
@@ -1467,7 +1534,7 @@
         <v>1.8181818181818181E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>56.5</v>
       </c>
@@ -1484,7 +1551,7 @@
         <v>0.14545454545454545</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>52.5</v>
       </c>
@@ -1501,7 +1568,7 @@
         <v>0.30909090909090908</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <v>47</v>
       </c>
@@ -1515,7 +1582,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>82.4</v>
       </c>
@@ -1529,7 +1596,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>96</v>
       </c>
@@ -1543,7 +1610,7 @@
         <v>0.70909090909090911</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>64</v>
       </c>
@@ -1557,7 +1624,7 @@
         <v>0.76363636363636367</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>46</v>
       </c>
@@ -1571,7 +1638,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="15">
         <v>33</v>
       </c>
@@ -1585,213 +1652,213 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>58.17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <v>34.17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <v>47.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <v>42.75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="15">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <v>71.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="15">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <v>61.5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <v>71.5</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <v>43.5</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="15">
         <v>108.5</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <f>87*2</f>
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <f>29+33</f>
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <f>40+39</f>
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <f>75+50</f>
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <v>104.5</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <f>75+71</f>
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <v>131.5</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D8:D16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D8:D16">
     <sortCondition ref="D8"/>
   </sortState>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Liste an FotografInnen wird angezeigt, das Fenster lässt sich vergrößern und verkleiner, Details von FotografInnen wird angezeigt
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6923A2-8A55-4641-A35D-4368AB2E8B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E418C0-0491-4DB2-A6EC-3484B5983B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1870" yWindow="0" windowWidth="18280" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="140" windowWidth="13720" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notenrechner" sheetId="2" r:id="rId1"/>
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1205,7 +1205,9 @@
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
@@ -1215,7 +1217,9 @@
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
       <c r="C9" s="7">
         <v>2</v>
       </c>
@@ -1226,7 +1230,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="7">
         <v>2</v>
@@ -1313,7 +1317,9 @@
       <c r="A21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
       <c r="C21" s="7">
         <v>1</v>
       </c>
@@ -1351,7 +1357,9 @@
       <c r="A26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
       <c r="C26" s="7">
         <v>1</v>
       </c>
@@ -1405,7 +1413,7 @@
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>

</xml_diff>

<commit_message>
FotografInnen bearbeiten und validieren
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E418C0-0491-4DB2-A6EC-3484B5983B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF4BE1D-6166-4449-BC4A-A41EBEBA1DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="140" windowWidth="13720" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1241,7 +1241,9 @@
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
       <c r="C11" s="7">
         <v>1</v>
       </c>
@@ -1259,7 +1261,9 @@
       <c r="A14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
       <c r="C14" s="7">
         <v>1</v>
       </c>
@@ -1269,7 +1273,9 @@
       <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
       <c r="C15" s="7">
         <v>2</v>
       </c>
@@ -1289,7 +1295,9 @@
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
@@ -1299,7 +1307,9 @@
       <c r="A18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
@@ -1413,7 +1423,7 @@
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>

</xml_diff>

<commit_message>
Bilder können FotografInnen zugeordnet werden
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF4BE1D-6166-4449-BC4A-A41EBEBA1DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DD3F59-E752-4FCE-9A6C-D5C7AF3574D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="140" windowWidth="13720" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <definedName name="TabelleNotenTest">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1134,7 +1135,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,7 +1286,9 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
@@ -1423,7 +1426,7 @@
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>

</xml_diff>

<commit_message>
Tags können bearbeitet, hinzugefügt und entfernt werden. Design bei FotografInnen und Informationen verbessert
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DD3F59-E752-4FCE-9A6C-D5C7AF3574D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D945C3-4660-4814-943D-10D9FD995BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="140" windowWidth="13720" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1342,7 +1342,9 @@
       <c r="A22" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
       <c r="C22" s="7">
         <v>1</v>
       </c>
@@ -1426,7 +1428,7 @@
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>

</xml_diff>

<commit_message>
EXIF Daten können bearbeitet werden, alle Ansichten werden in Anzeigen und Bearbeiten geteilt, die Daten werden im ViewModel gesetzt, UserFeedback beim Bearbeiten
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D945C3-4660-4814-943D-10D9FD995BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E656A36-DE67-414B-91F0-2696CA87583F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="140" windowWidth="13720" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,7 +1362,9 @@
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
       <c r="C25" s="7">
         <v>2</v>
       </c>
@@ -1428,7 +1430,7 @@
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>

</xml_diff>